<commit_message>
spefic search function sorted
</commit_message>
<xml_diff>
--- a/db/database.xlsx
+++ b/db/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/NAVRAJ MAC BACKUP_2024-12-12/DATA/SAIT-IDD-Graphics Design Major/2nd Year/SEM 2/PROJ-309-Capstone Project/PROJECT SAIT CONNECT/Website/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E5FC4D-C351-0C42-9B97-6F62042DA928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CA27C-724E-924F-BC43-EACA9B7E84AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8900" yWindow="6200" windowWidth="27100" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7893,8 +7893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18:N60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20:AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9071,5 +9071,6 @@
     <hyperlink ref="F41" r:id="rId3" xr:uid="{3DAC51BC-DB66-844B-8A06-FFD743046832}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed email to teams for the connect button
</commit_message>
<xml_diff>
--- a/db/database.xlsx
+++ b/db/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/NAVRAJ MAC BACKUP_2024-12-12/DATA/SAIT-IDD-Graphics Design Major/2nd Year/SEM 2/PROJ-309-Capstone Project/PROJECT SAIT CONNECT/Website/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CA27C-724E-924F-BC43-EACA9B7E84AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1823F3C8-3C7A-F943-A5E0-D2B16425E61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8900" yWindow="6200" windowWidth="27100" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -7454,6 +7454,15 @@
   </si>
   <si>
     <t xml:space="preserve">// </t>
+  </si>
+  <si>
+    <t>Pronoun</t>
+  </si>
+  <si>
+    <t>He/Him</t>
+  </si>
+  <si>
+    <t>She/Her</t>
   </si>
 </sst>
 </file>
@@ -7579,7 +7588,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -7893,8 +7902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:AC37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7906,7 +7915,7 @@
     <col min="5" max="5" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7925,8 +7934,11 @@
       <c r="F1" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7945,8 +7957,11 @@
       <c r="F2" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -7963,7 +7978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -7980,7 +7995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -7997,7 +8012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8014,7 +8029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -8031,7 +8046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -8048,7 +8063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -8065,7 +8080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -8082,7 +8097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -8099,7 +8114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -8116,7 +8131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -8133,7 +8148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -8150,7 +8165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -8167,7 +8182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8280,6 +8295,9 @@
       <c r="F21" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
       <c r="N21" s="6" t="s">
         <v>79</v>
       </c>
@@ -8682,6 +8700,9 @@
       </c>
       <c r="F41" s="3" t="s">
         <v>74</v>
+      </c>
+      <c r="G41" t="s">
+        <v>120</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>99</v>

</xml_diff>